<commit_message>
Finished classification on Full VPOP with 1%, 5% and 10% uniform noise
</commit_message>
<xml_diff>
--- a/Classification Results/Augmented Data/Full VPOP Classification/By Diagnosis/Full VPOP Classification Summary.xlsx
+++ b/Classification Results/Augmented Data/Full VPOP Classification/By Diagnosis/Full VPOP Classification Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher/Documents/PTSD/NCDE Model/Classification Results/Augmented Data/Full VPOP Classification/By Diagnosis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFBD2D6-1F3F-EF4D-BCDC-924DC6236B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10BC257-859C-B64D-8AA6-45478507CA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="500" windowWidth="14400" windowHeight="16660" xr2:uid="{064A12D9-DF30-0A45-B172-879C6B680B9E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="32">
   <si>
     <t>Control</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Total Incorrect</t>
+  </si>
+  <si>
+    <t>Uniform Noise - 1%</t>
   </si>
 </sst>
 </file>
@@ -321,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -349,12 +352,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,7 +361,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF02A33-AEE7-C74D-B125-3664DD3F27B5}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,37 +714,37 @@
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="D3" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M3" s="15" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="10" t="s">
@@ -752,24 +756,24 @@
         <v>1</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
@@ -1369,37 +1373,37 @@
       <c r="B21" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="19" t="s">
+      <c r="D21" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="17" t="s">
+      <c r="K21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M21" s="17" t="s">
+      <c r="M21" s="15" t="s">
         <v>12</v>
       </c>
       <c r="N21" s="10" t="s">
@@ -1411,24 +1415,24 @@
         <v>1</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
       <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="5">
         <v>4</v>
       </c>
@@ -2031,37 +2035,37 @@
       <c r="B40" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J40" s="19" t="s">
+      <c r="D40" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K40" s="17" t="s">
+      <c r="K40" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="L40" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M40" s="17" t="s">
+      <c r="M40" s="15" t="s">
         <v>12</v>
       </c>
       <c r="N40" s="10" t="s">
@@ -2073,24 +2077,24 @@
         <v>1</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16"/>
+      <c r="M41" s="16"/>
       <c r="N41" s="12"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="16"/>
+      <c r="B42" s="19"/>
       <c r="C42" s="5">
         <v>6</v>
       </c>
@@ -2690,37 +2694,37 @@
       <c r="B58" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C58" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D58" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I58" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J58" s="19" t="s">
+      <c r="D58" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G58" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I58" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="K58" s="17" t="s">
+      <c r="K58" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="L58" s="19" t="s">
+      <c r="L58" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="M58" s="17" t="s">
+      <c r="M58" s="15" t="s">
         <v>12</v>
       </c>
       <c r="N58" s="10" t="s">
@@ -2732,24 +2736,24 @@
         <v>1</v>
       </c>
       <c r="B59" s="2"/>
-      <c r="C59" s="18"/>
-      <c r="D59" s="18"/>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="18"/>
-      <c r="L59" s="18"/>
-      <c r="M59" s="18"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16"/>
+      <c r="M59" s="16"/>
       <c r="N59" s="12"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="16"/>
+      <c r="B60" s="19"/>
       <c r="C60" s="5">
         <v>5</v>
       </c>
@@ -3316,6 +3320,8 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
       <c r="M73" t="s">
         <v>29</v>
       </c>
@@ -3325,6 +3331,8 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
       <c r="M74" t="s">
         <v>30</v>
       </c>
@@ -3333,8 +3341,1329 @@
         <v>481</v>
       </c>
     </row>
+    <row r="75" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="20"/>
+      <c r="C75" s="20"/>
+    </row>
+    <row r="76" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+    </row>
+    <row r="77" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="A77" s="1"/>
+      <c r="B77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I77" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J77" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K77" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L77" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M77" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N77" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="16"/>
+      <c r="D78" s="16"/>
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="16"/>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="16"/>
+      <c r="L78" s="16"/>
+      <c r="M78" s="16"/>
+      <c r="N78" s="12"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B79" s="19"/>
+      <c r="C79" s="5">
+        <v>6</v>
+      </c>
+      <c r="D79" s="3">
+        <v>5</v>
+      </c>
+      <c r="E79" s="5">
+        <v>3</v>
+      </c>
+      <c r="F79" s="3">
+        <v>5</v>
+      </c>
+      <c r="G79" s="5">
+        <v>6</v>
+      </c>
+      <c r="H79" s="3">
+        <v>6</v>
+      </c>
+      <c r="I79" s="5">
+        <v>6</v>
+      </c>
+      <c r="J79" s="3">
+        <v>3</v>
+      </c>
+      <c r="K79" s="5">
+        <v>4</v>
+      </c>
+      <c r="L79" s="3">
+        <v>4</v>
+      </c>
+      <c r="M79" s="5">
+        <v>3</v>
+      </c>
+      <c r="N79" s="5">
+        <f>SUM(C79:M79)/107</f>
+        <v>0.47663551401869159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A80" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" s="11"/>
+      <c r="C80" s="6">
+        <v>7</v>
+      </c>
+      <c r="D80">
+        <v>6</v>
+      </c>
+      <c r="E80" s="6">
+        <v>5</v>
+      </c>
+      <c r="F80" s="6">
+        <v>7</v>
+      </c>
+      <c r="G80" s="6">
+        <v>7</v>
+      </c>
+      <c r="H80" s="6">
+        <v>8</v>
+      </c>
+      <c r="I80" s="6">
+        <v>7</v>
+      </c>
+      <c r="J80" s="6">
+        <v>5</v>
+      </c>
+      <c r="K80" s="6">
+        <v>5</v>
+      </c>
+      <c r="L80" s="6">
+        <v>8</v>
+      </c>
+      <c r="M80" s="6">
+        <v>4</v>
+      </c>
+      <c r="N80" s="5">
+        <f t="shared" ref="N80:N89" si="17">SUM(C80:M80)/107</f>
+        <v>0.64485981308411211</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B81" s="11"/>
+      <c r="C81" s="6">
+        <v>7</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81" s="6">
+        <v>6</v>
+      </c>
+      <c r="F81" s="6">
+        <v>9</v>
+      </c>
+      <c r="G81" s="6">
+        <v>9</v>
+      </c>
+      <c r="H81" s="6">
+        <v>9</v>
+      </c>
+      <c r="I81" s="6">
+        <v>7</v>
+      </c>
+      <c r="J81" s="6">
+        <v>7</v>
+      </c>
+      <c r="K81" s="6">
+        <v>7</v>
+      </c>
+      <c r="L81" s="6">
+        <v>7</v>
+      </c>
+      <c r="M81" s="6">
+        <v>5</v>
+      </c>
+      <c r="N81" s="5">
+        <f t="shared" si="17"/>
+        <v>0.71962616822429903</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A82" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="11"/>
+      <c r="C82" s="6">
+        <v>6</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+      <c r="E82" s="6">
+        <v>5</v>
+      </c>
+      <c r="F82" s="6">
+        <v>7</v>
+      </c>
+      <c r="G82" s="6">
+        <v>7</v>
+      </c>
+      <c r="H82" s="6">
+        <v>6</v>
+      </c>
+      <c r="I82" s="6">
+        <v>5</v>
+      </c>
+      <c r="J82" s="6">
+        <v>4</v>
+      </c>
+      <c r="K82" s="6">
+        <v>4</v>
+      </c>
+      <c r="L82" s="6">
+        <v>6</v>
+      </c>
+      <c r="M82" s="6">
+        <v>3</v>
+      </c>
+      <c r="N82" s="5">
+        <f t="shared" si="17"/>
+        <v>0.54205607476635509</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A83" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="11"/>
+      <c r="C83" s="6">
+        <v>6</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83" s="6">
+        <v>6</v>
+      </c>
+      <c r="F83" s="6">
+        <v>7</v>
+      </c>
+      <c r="G83" s="6">
+        <v>7</v>
+      </c>
+      <c r="H83" s="6">
+        <v>7</v>
+      </c>
+      <c r="I83" s="6">
+        <v>6</v>
+      </c>
+      <c r="J83" s="6">
+        <v>6</v>
+      </c>
+      <c r="K83" s="6">
+        <v>3</v>
+      </c>
+      <c r="L83" s="6">
+        <v>9</v>
+      </c>
+      <c r="M83" s="6">
+        <v>4</v>
+      </c>
+      <c r="N83" s="5">
+        <f t="shared" si="17"/>
+        <v>0.61682242990654201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A84" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="11"/>
+      <c r="C84" s="6">
+        <v>8</v>
+      </c>
+      <c r="D84">
+        <v>4</v>
+      </c>
+      <c r="E84" s="6">
+        <v>5</v>
+      </c>
+      <c r="F84" s="6">
+        <v>7</v>
+      </c>
+      <c r="G84" s="6">
+        <v>7</v>
+      </c>
+      <c r="H84" s="6">
+        <v>8</v>
+      </c>
+      <c r="I84" s="6">
+        <v>6</v>
+      </c>
+      <c r="J84" s="6">
+        <v>5</v>
+      </c>
+      <c r="K84" s="6">
+        <v>3</v>
+      </c>
+      <c r="L84" s="6">
+        <v>9</v>
+      </c>
+      <c r="M84" s="6">
+        <v>4</v>
+      </c>
+      <c r="N84" s="5">
+        <f t="shared" si="17"/>
+        <v>0.61682242990654201</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B85" s="11"/>
+      <c r="C85" s="6">
+        <v>5</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85" s="6">
+        <v>5</v>
+      </c>
+      <c r="F85" s="6">
+        <v>5</v>
+      </c>
+      <c r="G85" s="6">
+        <v>8</v>
+      </c>
+      <c r="H85" s="6">
+        <v>7</v>
+      </c>
+      <c r="I85" s="6">
+        <v>4</v>
+      </c>
+      <c r="J85" s="6">
+        <v>5</v>
+      </c>
+      <c r="K85" s="6">
+        <v>2</v>
+      </c>
+      <c r="L85" s="6">
+        <v>7</v>
+      </c>
+      <c r="M85" s="6">
+        <v>3</v>
+      </c>
+      <c r="N85" s="5">
+        <f t="shared" si="17"/>
+        <v>0.51401869158878499</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A86" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" s="11"/>
+      <c r="C86" s="6">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>6</v>
+      </c>
+      <c r="E86" s="6">
+        <v>3</v>
+      </c>
+      <c r="F86" s="6">
+        <v>7</v>
+      </c>
+      <c r="G86" s="6">
+        <v>8</v>
+      </c>
+      <c r="H86" s="6">
+        <v>5</v>
+      </c>
+      <c r="I86" s="6">
+        <v>6</v>
+      </c>
+      <c r="J86" s="6">
+        <v>4</v>
+      </c>
+      <c r="K86" s="6">
+        <v>4</v>
+      </c>
+      <c r="L86" s="6">
+        <v>7</v>
+      </c>
+      <c r="M86" s="6">
+        <v>4</v>
+      </c>
+      <c r="N86" s="5">
+        <f t="shared" si="17"/>
+        <v>0.55140186915887845</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A87" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B87" s="11"/>
+      <c r="C87" s="6">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87" s="6">
+        <v>5</v>
+      </c>
+      <c r="F87" s="6">
+        <v>8</v>
+      </c>
+      <c r="G87" s="6">
+        <v>8</v>
+      </c>
+      <c r="H87" s="6">
+        <v>8</v>
+      </c>
+      <c r="I87" s="6">
+        <v>8</v>
+      </c>
+      <c r="J87" s="6">
+        <v>6</v>
+      </c>
+      <c r="K87" s="6">
+        <v>5</v>
+      </c>
+      <c r="L87" s="6">
+        <v>8</v>
+      </c>
+      <c r="M87" s="6">
+        <v>5</v>
+      </c>
+      <c r="N87" s="5">
+        <f t="shared" si="17"/>
+        <v>0.67289719626168221</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A88" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B88" s="11"/>
+      <c r="C88" s="6">
+        <v>6</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+      <c r="E88" s="6">
+        <v>3</v>
+      </c>
+      <c r="F88" s="6">
+        <v>6</v>
+      </c>
+      <c r="G88" s="6">
+        <v>6</v>
+      </c>
+      <c r="H88" s="6">
+        <v>6</v>
+      </c>
+      <c r="I88" s="6">
+        <v>5</v>
+      </c>
+      <c r="J88" s="6">
+        <v>5</v>
+      </c>
+      <c r="K88" s="6">
+        <v>6</v>
+      </c>
+      <c r="L88" s="6">
+        <v>6</v>
+      </c>
+      <c r="M88" s="6">
+        <v>3</v>
+      </c>
+      <c r="N88" s="5">
+        <f t="shared" si="17"/>
+        <v>0.52336448598130836</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" s="11"/>
+      <c r="C89" s="6">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>5</v>
+      </c>
+      <c r="E89" s="6">
+        <v>5</v>
+      </c>
+      <c r="F89" s="6">
+        <v>8</v>
+      </c>
+      <c r="G89" s="6">
+        <v>8</v>
+      </c>
+      <c r="H89" s="6">
+        <v>8</v>
+      </c>
+      <c r="I89" s="6">
+        <v>7</v>
+      </c>
+      <c r="J89" s="6">
+        <v>6</v>
+      </c>
+      <c r="K89" s="6">
+        <v>6</v>
+      </c>
+      <c r="L89" s="6">
+        <v>7</v>
+      </c>
+      <c r="M89" s="6">
+        <v>5</v>
+      </c>
+      <c r="N89" s="5">
+        <f t="shared" si="17"/>
+        <v>0.64485981308411211</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A90" s="12">
+        <v>2</v>
+      </c>
+      <c r="B90" s="13"/>
+      <c r="C90" s="7">
+        <v>4</v>
+      </c>
+      <c r="D90" s="4">
+        <v>4</v>
+      </c>
+      <c r="E90" s="7">
+        <v>3</v>
+      </c>
+      <c r="F90" s="4">
+        <v>5</v>
+      </c>
+      <c r="G90" s="7">
+        <v>5</v>
+      </c>
+      <c r="H90" s="4">
+        <v>5</v>
+      </c>
+      <c r="I90" s="7">
+        <v>3</v>
+      </c>
+      <c r="J90" s="4">
+        <v>3</v>
+      </c>
+      <c r="K90" s="7">
+        <v>3</v>
+      </c>
+      <c r="L90" s="4">
+        <v>5</v>
+      </c>
+      <c r="M90" s="7">
+        <v>2</v>
+      </c>
+      <c r="N90" s="5">
+        <f>SUM(C90:M90)/63</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A91" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="8">
+        <f>SUM(C79:C90)/116</f>
+        <v>0.60344827586206895</v>
+      </c>
+      <c r="D91" s="8">
+        <f t="shared" ref="D91:L91" si="18">SUM(D79:D90)/116</f>
+        <v>0.49137931034482757</v>
+      </c>
+      <c r="E91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.46551724137931033</v>
+      </c>
+      <c r="F91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.69827586206896552</v>
+      </c>
+      <c r="G91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.74137931034482762</v>
+      </c>
+      <c r="H91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.71551724137931039</v>
+      </c>
+      <c r="I91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.60344827586206895</v>
+      </c>
+      <c r="J91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.50862068965517238</v>
+      </c>
+      <c r="K91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.44827586206896552</v>
+      </c>
+      <c r="L91" s="8">
+        <f t="shared" si="18"/>
+        <v>0.71551724137931039</v>
+      </c>
+      <c r="M91" s="8">
+        <f>SUM(M79:M90)/80</f>
+        <v>0.5625</v>
+      </c>
+      <c r="N91">
+        <f>SUM(C79:M90)/1240</f>
+        <v>0.59677419354838712</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="M92" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92">
+        <f>SUM(C79:M90)</f>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="M93" t="s">
+        <v>30</v>
+      </c>
+      <c r="N93">
+        <f>SUM(-N92, 1240)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A94" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B94" s="20"/>
+      <c r="C94" s="20"/>
+    </row>
+    <row r="95" spans="1:14" ht="26" x14ac:dyDescent="0.3">
+      <c r="A95" s="1"/>
+      <c r="B95" t="s">
+        <v>0</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G95" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="I95" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J95" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="K95" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L95" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M95" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N95" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="C96" s="16"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="16"/>
+      <c r="M96" s="16"/>
+      <c r="N96" s="12"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B97" s="19"/>
+      <c r="C97" s="5">
+        <v>7</v>
+      </c>
+      <c r="D97" s="3">
+        <v>6</v>
+      </c>
+      <c r="E97" s="5">
+        <v>3</v>
+      </c>
+      <c r="F97" s="3">
+        <v>6</v>
+      </c>
+      <c r="G97" s="5">
+        <v>7</v>
+      </c>
+      <c r="H97" s="3">
+        <v>4</v>
+      </c>
+      <c r="I97" s="5">
+        <v>6</v>
+      </c>
+      <c r="J97" s="3">
+        <v>3</v>
+      </c>
+      <c r="K97" s="5">
+        <v>3</v>
+      </c>
+      <c r="L97" s="3">
+        <v>4</v>
+      </c>
+      <c r="M97" s="5">
+        <v>2</v>
+      </c>
+      <c r="N97" s="5">
+        <f>SUM(C97:M97)/107</f>
+        <v>0.47663551401869159</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B98" s="11"/>
+      <c r="C98" s="6">
+        <v>7</v>
+      </c>
+      <c r="D98">
+        <v>5</v>
+      </c>
+      <c r="E98" s="6">
+        <v>5</v>
+      </c>
+      <c r="F98" s="6">
+        <v>4</v>
+      </c>
+      <c r="G98" s="6">
+        <v>7</v>
+      </c>
+      <c r="H98" s="6">
+        <v>8</v>
+      </c>
+      <c r="I98" s="6">
+        <v>6</v>
+      </c>
+      <c r="J98" s="6">
+        <v>5</v>
+      </c>
+      <c r="K98" s="6">
+        <v>5</v>
+      </c>
+      <c r="L98" s="6">
+        <v>7</v>
+      </c>
+      <c r="M98" s="6">
+        <v>4</v>
+      </c>
+      <c r="N98" s="5">
+        <f t="shared" ref="N98:N107" si="19">SUM(C98:M98)/107</f>
+        <v>0.58878504672897192</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B99" s="11"/>
+      <c r="C99" s="6">
+        <v>7</v>
+      </c>
+      <c r="D99">
+        <v>4</v>
+      </c>
+      <c r="E99" s="6">
+        <v>6</v>
+      </c>
+      <c r="F99" s="6">
+        <v>9</v>
+      </c>
+      <c r="G99" s="6">
+        <v>9</v>
+      </c>
+      <c r="H99" s="6">
+        <v>8</v>
+      </c>
+      <c r="I99" s="6">
+        <v>7</v>
+      </c>
+      <c r="J99" s="6">
+        <v>7</v>
+      </c>
+      <c r="K99" s="6">
+        <v>6</v>
+      </c>
+      <c r="L99" s="6">
+        <v>9</v>
+      </c>
+      <c r="M99" s="6">
+        <v>6</v>
+      </c>
+      <c r="N99" s="5">
+        <f t="shared" si="19"/>
+        <v>0.7289719626168224</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B100" s="11"/>
+      <c r="C100" s="6">
+        <v>6</v>
+      </c>
+      <c r="D100">
+        <v>4</v>
+      </c>
+      <c r="E100" s="6">
+        <v>4</v>
+      </c>
+      <c r="F100" s="6">
+        <v>7</v>
+      </c>
+      <c r="G100" s="6">
+        <v>7</v>
+      </c>
+      <c r="H100" s="6">
+        <v>7</v>
+      </c>
+      <c r="I100" s="6">
+        <v>6</v>
+      </c>
+      <c r="J100" s="6">
+        <v>4</v>
+      </c>
+      <c r="K100" s="6">
+        <v>5</v>
+      </c>
+      <c r="L100" s="6">
+        <v>4</v>
+      </c>
+      <c r="M100" s="6">
+        <v>3</v>
+      </c>
+      <c r="N100" s="5">
+        <f t="shared" si="19"/>
+        <v>0.53271028037383172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B101" s="11"/>
+      <c r="C101" s="6">
+        <v>6</v>
+      </c>
+      <c r="D101">
+        <v>5</v>
+      </c>
+      <c r="E101" s="6">
+        <v>4</v>
+      </c>
+      <c r="F101" s="6">
+        <v>7</v>
+      </c>
+      <c r="G101" s="6">
+        <v>8</v>
+      </c>
+      <c r="H101" s="6">
+        <v>8</v>
+      </c>
+      <c r="I101" s="6">
+        <v>6</v>
+      </c>
+      <c r="J101" s="6">
+        <v>5</v>
+      </c>
+      <c r="K101" s="6">
+        <v>4</v>
+      </c>
+      <c r="L101" s="6">
+        <v>8</v>
+      </c>
+      <c r="M101" s="6">
+        <v>4</v>
+      </c>
+      <c r="N101" s="5">
+        <f t="shared" si="19"/>
+        <v>0.60747663551401865</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B102" s="11"/>
+      <c r="C102" s="6">
+        <v>7</v>
+      </c>
+      <c r="D102">
+        <v>5</v>
+      </c>
+      <c r="E102" s="6">
+        <v>5</v>
+      </c>
+      <c r="F102" s="6">
+        <v>7</v>
+      </c>
+      <c r="G102" s="6">
+        <v>5</v>
+      </c>
+      <c r="H102" s="6">
+        <v>7</v>
+      </c>
+      <c r="I102" s="6">
+        <v>5</v>
+      </c>
+      <c r="J102" s="6">
+        <v>5</v>
+      </c>
+      <c r="K102" s="6">
+        <v>4</v>
+      </c>
+      <c r="L102" s="6">
+        <v>8</v>
+      </c>
+      <c r="M102" s="6">
+        <v>4</v>
+      </c>
+      <c r="N102" s="5">
+        <f t="shared" si="19"/>
+        <v>0.57943925233644855</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B103" s="11"/>
+      <c r="C103" s="6">
+        <v>5</v>
+      </c>
+      <c r="D103">
+        <v>4</v>
+      </c>
+      <c r="E103" s="6">
+        <v>5</v>
+      </c>
+      <c r="F103" s="6">
+        <v>6</v>
+      </c>
+      <c r="G103" s="6">
+        <v>7</v>
+      </c>
+      <c r="H103" s="6">
+        <v>7</v>
+      </c>
+      <c r="I103" s="6">
+        <v>6</v>
+      </c>
+      <c r="J103" s="6">
+        <v>5</v>
+      </c>
+      <c r="K103" s="6">
+        <v>4</v>
+      </c>
+      <c r="L103" s="6">
+        <v>6</v>
+      </c>
+      <c r="M103" s="6">
+        <v>5</v>
+      </c>
+      <c r="N103" s="5">
+        <f t="shared" si="19"/>
+        <v>0.56074766355140182</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A104" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B104" s="11"/>
+      <c r="C104" s="6">
+        <v>5</v>
+      </c>
+      <c r="D104">
+        <v>6</v>
+      </c>
+      <c r="E104" s="6">
+        <v>4</v>
+      </c>
+      <c r="F104" s="6">
+        <v>7</v>
+      </c>
+      <c r="G104" s="6">
+        <v>6</v>
+      </c>
+      <c r="H104" s="6">
+        <v>6</v>
+      </c>
+      <c r="I104" s="6">
+        <v>7</v>
+      </c>
+      <c r="J104" s="6">
+        <v>5</v>
+      </c>
+      <c r="K104" s="6">
+        <v>3</v>
+      </c>
+      <c r="L104" s="6">
+        <v>7</v>
+      </c>
+      <c r="M104" s="6">
+        <v>4</v>
+      </c>
+      <c r="N104" s="5">
+        <f t="shared" si="19"/>
+        <v>0.56074766355140182</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A105" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B105" s="11"/>
+      <c r="C105" s="6">
+        <v>7</v>
+      </c>
+      <c r="D105">
+        <v>4</v>
+      </c>
+      <c r="E105" s="6">
+        <v>5</v>
+      </c>
+      <c r="F105" s="6">
+        <v>8</v>
+      </c>
+      <c r="G105" s="6">
+        <v>8</v>
+      </c>
+      <c r="H105" s="6">
+        <v>7</v>
+      </c>
+      <c r="I105" s="6">
+        <v>7</v>
+      </c>
+      <c r="J105" s="6">
+        <v>6</v>
+      </c>
+      <c r="K105" s="6">
+        <v>4</v>
+      </c>
+      <c r="L105" s="6">
+        <v>7</v>
+      </c>
+      <c r="M105" s="6">
+        <v>5</v>
+      </c>
+      <c r="N105" s="5">
+        <f t="shared" si="19"/>
+        <v>0.63551401869158874</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A106" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B106" s="11"/>
+      <c r="C106" s="6">
+        <v>7</v>
+      </c>
+      <c r="D106">
+        <v>5</v>
+      </c>
+      <c r="E106" s="6">
+        <v>3</v>
+      </c>
+      <c r="F106" s="6">
+        <v>6</v>
+      </c>
+      <c r="G106" s="6">
+        <v>7</v>
+      </c>
+      <c r="H106" s="6">
+        <v>6</v>
+      </c>
+      <c r="I106" s="6">
+        <v>6</v>
+      </c>
+      <c r="J106" s="6">
+        <v>5</v>
+      </c>
+      <c r="K106" s="6">
+        <v>6</v>
+      </c>
+      <c r="L106" s="6">
+        <v>6</v>
+      </c>
+      <c r="M106" s="6">
+        <v>3</v>
+      </c>
+      <c r="N106" s="5">
+        <f t="shared" si="19"/>
+        <v>0.56074766355140182</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A107" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="11"/>
+      <c r="C107" s="6">
+        <v>6</v>
+      </c>
+      <c r="D107">
+        <v>4</v>
+      </c>
+      <c r="E107" s="6">
+        <v>5</v>
+      </c>
+      <c r="F107" s="6">
+        <v>8</v>
+      </c>
+      <c r="G107" s="6">
+        <v>8</v>
+      </c>
+      <c r="H107" s="6">
+        <v>7</v>
+      </c>
+      <c r="I107" s="21">
+        <v>8</v>
+      </c>
+      <c r="J107" s="6">
+        <v>6</v>
+      </c>
+      <c r="K107" s="6">
+        <v>5</v>
+      </c>
+      <c r="L107" s="6">
+        <v>7</v>
+      </c>
+      <c r="M107" s="6">
+        <v>5</v>
+      </c>
+      <c r="N107" s="5">
+        <f t="shared" si="19"/>
+        <v>0.64485981308411211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A108" s="12">
+        <v>2</v>
+      </c>
+      <c r="B108" s="13"/>
+      <c r="C108" s="7">
+        <v>4</v>
+      </c>
+      <c r="D108" s="4">
+        <v>4</v>
+      </c>
+      <c r="E108" s="7">
+        <v>2</v>
+      </c>
+      <c r="F108" s="4">
+        <v>4</v>
+      </c>
+      <c r="G108" s="7">
+        <v>5</v>
+      </c>
+      <c r="H108" s="4">
+        <v>5</v>
+      </c>
+      <c r="I108" s="7">
+        <v>3</v>
+      </c>
+      <c r="J108" s="4">
+        <v>2</v>
+      </c>
+      <c r="K108" s="7">
+        <v>2</v>
+      </c>
+      <c r="L108" s="4">
+        <v>6</v>
+      </c>
+      <c r="M108" s="7">
+        <v>2</v>
+      </c>
+      <c r="N108" s="5">
+        <f>SUM(C108:M108)/63</f>
+        <v>0.61904761904761907</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A109" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" s="14"/>
+      <c r="C109" s="8">
+        <f>SUM(C97:C108)/116</f>
+        <v>0.63793103448275867</v>
+      </c>
+      <c r="D109" s="8">
+        <f t="shared" ref="D109:L109" si="20">SUM(D97:D108)/116</f>
+        <v>0.48275862068965519</v>
+      </c>
+      <c r="E109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.43965517241379309</v>
+      </c>
+      <c r="F109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.68103448275862066</v>
+      </c>
+      <c r="G109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.72413793103448276</v>
+      </c>
+      <c r="H109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.68965517241379315</v>
+      </c>
+      <c r="I109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.62931034482758619</v>
+      </c>
+      <c r="J109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="K109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.43965517241379309</v>
+      </c>
+      <c r="L109" s="8">
+        <f t="shared" si="20"/>
+        <v>0.68103448275862066</v>
+      </c>
+      <c r="M109" s="8">
+        <f>SUM(M97:M108)/80</f>
+        <v>0.58750000000000002</v>
+      </c>
+      <c r="N109" s="8">
+        <f>SUM(C97:M108)/1240</f>
+        <v>0.5903225806451613</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M110" t="s">
+        <v>29</v>
+      </c>
+      <c r="N110">
+        <f>SUM(C97:M108)</f>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M111" t="s">
+        <v>30</v>
+      </c>
+      <c r="N111">
+        <f>SUM(-N110, 1240)</f>
+        <v>508</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="159">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
@@ -3441,6 +4770,59 @@
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="A67:B67"/>
     <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A76:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="J77:J78"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="L77:L78"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="N77:N78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="L95:L96"/>
+    <mergeCell ref="M95:M96"/>
+    <mergeCell ref="N95:N96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A94:C94"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="D95:D96"/>
+    <mergeCell ref="E95:E96"/>
+    <mergeCell ref="F95:F96"/>
+    <mergeCell ref="G95:G96"/>
+    <mergeCell ref="H95:H96"/>
+    <mergeCell ref="I95:I96"/>
+    <mergeCell ref="J95:J96"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="K95:K96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>